<commit_message>
Update War Room: Manual v3, PDF fix, and dashboard enhancements
</commit_message>
<xml_diff>
--- a/dashboards_v2/CPO_Dashboard.xlsx
+++ b/dashboards_v2/CPO_Dashboard.xlsx
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1600</v>
+        <v>240</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="B5" s="18" t="inlineStr">
         <is>
-          <t>31200</t>
+          <t>12252</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B11" s="18" t="inlineStr">
         <is>
-          <t>LOW</t>
+          <t>🟡 Excess Cash</t>
         </is>
       </c>
     </row>

</xml_diff>